<commit_message>
Addition of final manually annotated files. Ready for evaluation.
</commit_message>
<xml_diff>
--- a/HLS_man/COP23/COP23_man_croatia.xlsx
+++ b/HLS_man/COP23/COP23_man_croatia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suze van Santen\Documents\GitHub\TextToDistributiveJustice\HLS_man\COP23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA32C20B-2930-4322-AC01-2309916F1340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABB069C-CAB4-4101-8F24-EB16BAF96F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,9 +144,6 @@
 Thank you for your attention.</t>
   </si>
   <si>
-    <t>ce</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t xml:space="preserve">Urging to take on action for the benefit of present and future generations. </t>
+  </si>
+  <si>
+    <t>COP23_croatia</t>
   </si>
 </sst>
 </file>
@@ -573,9 +573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -584,7 +582,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -616,7 +614,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -624,7 +622,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="72" x14ac:dyDescent="0.3">
@@ -632,7 +630,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
@@ -640,25 +638,25 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>29</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>30</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>31</v>
-      </c>
-      <c r="H5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
@@ -666,25 +664,25 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>35</v>
-      </c>
-      <c r="H6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -692,25 +690,25 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
         <v>37</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -718,25 +716,25 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
         <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -744,25 +742,25 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
         <v>41</v>
       </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>42</v>
-      </c>
-      <c r="H9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
@@ -770,7 +768,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
@@ -778,7 +776,7 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
@@ -786,7 +784,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
@@ -794,7 +792,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -802,7 +800,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -810,7 +808,7 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -818,7 +816,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -826,7 +824,7 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>